<commit_message>
Cleanup; Allow different base layers; Added KC_NONUS_BACKSLASH
</commit_message>
<xml_diff>
--- a/keyboards/handwired/polykybd/split72/keymaps/default/lang/lang_lut.xlsx
+++ b/keyboards/handwired/polykybd/split72/keymaps/default/lang/lang_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="named_glyphs" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="797">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -2355,24 +2355,21 @@
     <t xml:space="preserve">KC_NONUS_HASH</t>
   </si>
   <si>
+    <t xml:space="preserve">KC_SEMICOLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC_QUOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC_GRAVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\v\xb2</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;</t>
   </si>
   <si>
-    <t xml:space="preserve">KC_SEMICOLON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC_QUOTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KC_GRAVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\v\xb2</t>
-  </si>
-  <si>
     <t xml:space="preserve">KC_COMMA</t>
   </si>
   <si>
@@ -2383,6 +2380,12 @@
   </si>
   <si>
     <t xml:space="preserve">KC_SLASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC_NONUS_BACKSLASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;|</t>
   </si>
   <si>
     <t xml:space="preserve">lower</t>
@@ -2907,15 +2910,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2986,11 +2980,11 @@
   </sheetPr>
   <dimension ref="A1:G393"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A342" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A342" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D367" activeCellId="0" sqref="D367"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.74"/>
@@ -12357,19 +12351,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH115"/>
+  <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
-      <selection pane="bottomRight" activeCell="C79" activeCellId="0" sqref="C79"/>
+      <selection pane="bottomLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
+      <selection pane="bottomRight" activeCell="J67" activeCellId="0" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="18.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="21.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="14" width="16.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="15" width="16.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="16" width="16.9"/>
@@ -16855,94 +16849,32 @@
         <v>770</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>16</v>
+        <v>737</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>16</v>
+        <v>737</v>
       </c>
       <c r="E94" s="15" t="s">
-        <v>771</v>
+        <v>737</v>
       </c>
       <c r="F94" s="15" t="s">
-        <v>733</v>
-      </c>
-      <c r="H94" s="16" t="s">
-        <v>771</v>
-      </c>
-      <c r="I94" s="16" t="s">
-        <v>733</v>
-      </c>
-      <c r="K94" s="17" t="s">
-        <v>771</v>
-      </c>
-      <c r="L94" s="17" t="s">
-        <v>733</v>
-      </c>
-      <c r="M94" s="17" t="s">
-        <v>771</v>
-      </c>
-      <c r="N94" s="18" t="s">
-        <v>771</v>
-      </c>
-      <c r="O94" s="18" t="s">
-        <v>733</v>
-      </c>
-      <c r="P94" s="18" t="s">
-        <v>771</v>
-      </c>
-      <c r="Q94" s="19" t="s">
-        <v>771</v>
-      </c>
-      <c r="R94" s="19" t="s">
-        <v>733</v>
-      </c>
-      <c r="S94" s="19" t="s">
-        <v>771</v>
-      </c>
-      <c r="T94" s="20" t="s">
-        <v>771</v>
-      </c>
-      <c r="U94" s="20" t="s">
-        <v>733</v>
-      </c>
-      <c r="V94" s="20" t="s">
-        <v>771</v>
-      </c>
-      <c r="AC94" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD94" s="23" t="s">
-        <v>732</v>
-      </c>
-      <c r="AE94" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF94" s="24" t="s">
-        <v>733</v>
-      </c>
-      <c r="AG94" s="24" t="s">
-        <v>771</v>
-      </c>
-      <c r="AH94" s="24" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="95" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="38"/>
       <c r="B95" s="39" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="C95" s="39"/>
       <c r="D95" s="39"/>
       <c r="E95" s="40" t="s">
-        <v>732</v>
-      </c>
-      <c r="F95" s="40" t="s">
-        <v>732</v>
-      </c>
+        <v>735</v>
+      </c>
+      <c r="F95" s="40"/>
       <c r="G95" s="40"/>
       <c r="H95" s="41"/>
       <c r="I95" s="41"/>
@@ -16956,15 +16888,9 @@
       <c r="Q95" s="44"/>
       <c r="R95" s="44"/>
       <c r="S95" s="44"/>
-      <c r="T95" s="46" t="s">
-        <v>732</v>
-      </c>
-      <c r="U95" s="46" t="s">
-        <v>732</v>
-      </c>
-      <c r="V95" s="46" t="s">
-        <v>732</v>
-      </c>
+      <c r="T95" s="46"/>
+      <c r="U95" s="46"/>
+      <c r="V95" s="46"/>
       <c r="W95" s="47"/>
       <c r="X95" s="47"/>
       <c r="Y95" s="47"/>
@@ -16980,7 +16906,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="13" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B96" s="14" t="s">
         <v>695</v>
@@ -17108,7 +17034,7 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="13" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>735</v>
@@ -17189,10 +17115,12 @@
     <row r="99" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="38"/>
       <c r="B99" s="39" t="s">
-        <v>774</v>
+        <v>8</v>
       </c>
       <c r="C99" s="39"/>
-      <c r="D99" s="39"/>
+      <c r="D99" s="39" t="s">
+        <v>8</v>
+      </c>
       <c r="E99" s="40"/>
       <c r="F99" s="40"/>
       <c r="G99" s="40"/>
@@ -17238,7 +17166,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>18</v>
@@ -17259,13 +17187,13 @@
         <v>738</v>
       </c>
       <c r="H100" s="16" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="I100" s="16" t="s">
         <v>6</v>
       </c>
       <c r="J100" s="16" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="K100" s="66" t="s">
         <v>86</v>
@@ -17308,7 +17236,7 @@
         <v>733</v>
       </c>
       <c r="AD100" s="23" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="AE100" s="23" t="s">
         <v>733</v>
@@ -17352,10 +17280,10 @@
       <c r="R101" s="44"/>
       <c r="S101" s="44"/>
       <c r="T101" s="46" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="U101" s="46" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="V101" s="46"/>
       <c r="W101" s="47"/>
@@ -17373,17 +17301,20 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="D102" s="14" t="s">
         <v>10</v>
       </c>
+      <c r="E102" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="F102" s="15" t="s">
         <v>695</v>
       </c>
@@ -17391,34 +17322,34 @@
         <v>695</v>
       </c>
       <c r="I102" s="16" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="K102" s="17" t="s">
-        <v>682</v>
+        <v>10</v>
       </c>
       <c r="L102" s="17" t="s">
         <v>695</v>
       </c>
       <c r="M102" s="17" t="s">
-        <v>682</v>
+        <v>10</v>
       </c>
       <c r="N102" s="18" t="s">
-        <v>682</v>
+        <v>10</v>
       </c>
       <c r="O102" s="18" t="s">
         <v>695</v>
       </c>
       <c r="P102" s="18" t="s">
-        <v>682</v>
+        <v>10</v>
       </c>
       <c r="Q102" s="19" t="s">
-        <v>682</v>
+        <v>10</v>
       </c>
       <c r="R102" s="19" t="s">
         <v>695</v>
       </c>
       <c r="S102" s="19" t="s">
-        <v>682</v>
+        <v>10</v>
       </c>
       <c r="T102" s="20" t="s">
         <v>152</v>
@@ -17445,7 +17376,7 @@
         <v>10</v>
       </c>
       <c r="AG102" s="24" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="AH102" s="24" t="s">
         <v>10</v>
@@ -17454,11 +17385,15 @@
     <row r="103" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="38"/>
       <c r="B103" s="39" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="C103" s="39"/>
-      <c r="D103" s="39"/>
-      <c r="E103" s="40"/>
+      <c r="D103" s="39" t="s">
+        <v>775</v>
+      </c>
+      <c r="E103" s="40" t="s">
+        <v>695</v>
+      </c>
       <c r="F103" s="40"/>
       <c r="G103" s="40"/>
       <c r="H103" s="41"/>
@@ -17497,16 +17432,19 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="13" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C104" s="14" t="s">
         <v>733</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>778</v>
+        <v>777</v>
+      </c>
+      <c r="E104" s="15" t="s">
+        <v>777</v>
       </c>
       <c r="F104" s="15" t="s">
         <v>696</v>
@@ -17518,31 +17456,31 @@
         <v>678</v>
       </c>
       <c r="K104" s="17" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="L104" s="17" t="s">
         <v>696</v>
       </c>
       <c r="M104" s="17" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="N104" s="18" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="O104" s="18" t="s">
         <v>696</v>
       </c>
       <c r="P104" s="18" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="Q104" s="19" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="R104" s="19" t="s">
         <v>696</v>
       </c>
       <c r="S104" s="19" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="T104" s="20" t="s">
         <v>134</v>
@@ -17560,19 +17498,19 @@
         <v>306</v>
       </c>
       <c r="AD104" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AE104" s="23" t="s">
         <v>306</v>
       </c>
       <c r="AF104" s="24" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AG104" s="24" t="s">
         <v>733</v>
       </c>
       <c r="AH104" s="24" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="105" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17582,7 +17520,9 @@
       </c>
       <c r="C105" s="39"/>
       <c r="D105" s="39"/>
-      <c r="E105" s="40"/>
+      <c r="E105" s="40" t="s">
+        <v>696</v>
+      </c>
       <c r="F105" s="40"/>
       <c r="G105" s="40"/>
       <c r="H105" s="41"/>
@@ -17621,7 +17561,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="13" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B106" s="14" t="s">
         <v>678</v>
@@ -17675,13 +17615,13 @@
         <v>748</v>
       </c>
       <c r="T106" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="U106" s="20" t="s">
         <v>696</v>
       </c>
       <c r="V106" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="Z106" s="22" t="s">
         <v>527</v>
@@ -17723,258 +17663,249 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="67"/>
-      <c r="B108" s="67" t="s">
+      <c r="A108" s="13" t="s">
+        <v>780</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>775</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>733</v>
+      </c>
+      <c r="D108" s="14" t="s">
+        <v>775</v>
+      </c>
+      <c r="E108" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="F108" s="15" t="s">
+        <v>733</v>
+      </c>
+      <c r="H108" s="16" t="s">
+        <v>775</v>
+      </c>
+      <c r="I108" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="AC108" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD108" s="23" t="s">
+        <v>732</v>
+      </c>
+      <c r="AE108" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="38"/>
+      <c r="B109" s="39" t="s">
         <v>781</v>
       </c>
-      <c r="C108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="D108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="E108" s="67" t="s">
+      <c r="C109" s="39" t="s">
+        <v>732</v>
+      </c>
+      <c r="D109" s="39" t="s">
         <v>781</v>
       </c>
-      <c r="F108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="G108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="H108" s="67" t="s">
+      <c r="E109" s="40" t="s">
         <v>781</v>
       </c>
-      <c r="I108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="J108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="K108" s="67" t="s">
+      <c r="F109" s="40" t="s">
+        <v>732</v>
+      </c>
+      <c r="G109" s="40"/>
+      <c r="H109" s="41" t="s">
         <v>781</v>
       </c>
-      <c r="L108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="M108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="N108" s="67" t="s">
-        <v>781</v>
-      </c>
-      <c r="O108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="P108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="Q108" s="67" t="s">
-        <v>781</v>
-      </c>
-      <c r="R108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="S108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="T108" s="67" t="s">
-        <v>781</v>
-      </c>
-      <c r="U108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="V108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="W108" s="67" t="s">
-        <v>781</v>
-      </c>
-      <c r="X108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="Y108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="Z108" s="67" t="s">
-        <v>781</v>
-      </c>
-      <c r="AA108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="AB108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="AC108" s="67" t="s">
-        <v>781</v>
-      </c>
-      <c r="AD108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="AE108" s="67" t="s">
-        <v>783</v>
-      </c>
-      <c r="AF108" s="67" t="s">
-        <v>781</v>
-      </c>
-      <c r="AG108" s="67" t="s">
-        <v>782</v>
-      </c>
-      <c r="AH108" s="67" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="67"/>
-      <c r="B109" s="67"/>
-      <c r="C109" s="67"/>
-      <c r="D109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="E109" s="67"/>
-      <c r="F109" s="67"/>
-      <c r="G109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="H109" s="67"/>
-      <c r="I109" s="67"/>
-      <c r="J109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="K109" s="67"/>
-      <c r="L109" s="67"/>
-      <c r="M109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="N109" s="67"/>
-      <c r="O109" s="67"/>
-      <c r="P109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="Q109" s="67"/>
-      <c r="R109" s="67"/>
-      <c r="S109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="T109" s="67"/>
-      <c r="U109" s="67"/>
-      <c r="V109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="W109" s="67"/>
-      <c r="X109" s="67"/>
-      <c r="Y109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="Z109" s="67"/>
-      <c r="AA109" s="67"/>
-      <c r="AB109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="AC109" s="67"/>
-      <c r="AD109" s="67"/>
-      <c r="AE109" s="68" t="s">
-        <v>784</v>
-      </c>
-      <c r="AF109" s="67"/>
-      <c r="AG109" s="67"/>
-      <c r="AH109" s="68" t="s">
-        <v>784</v>
-      </c>
+      <c r="I109" s="41" t="s">
+        <v>732</v>
+      </c>
+      <c r="J109" s="41"/>
+      <c r="K109" s="42"/>
+      <c r="L109" s="42"/>
+      <c r="M109" s="42"/>
+      <c r="N109" s="43"/>
+      <c r="O109" s="43"/>
+      <c r="P109" s="43"/>
+      <c r="Q109" s="44"/>
+      <c r="R109" s="44"/>
+      <c r="S109" s="44"/>
+      <c r="T109" s="46"/>
+      <c r="U109" s="46"/>
+      <c r="V109" s="46"/>
+      <c r="W109" s="47"/>
+      <c r="X109" s="47"/>
+      <c r="Y109" s="47"/>
+      <c r="Z109" s="48"/>
+      <c r="AA109" s="48"/>
+      <c r="AB109" s="48"/>
+      <c r="AC109" s="49"/>
+      <c r="AD109" s="49"/>
+      <c r="AE109" s="49"/>
+      <c r="AF109" s="50"/>
+      <c r="AG109" s="50"/>
+      <c r="AH109" s="50"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="67"/>
-      <c r="B110" s="67"/>
-      <c r="C110" s="67"/>
-      <c r="D110" s="67"/>
-      <c r="E110" s="67"/>
-      <c r="F110" s="67"/>
-      <c r="G110" s="67"/>
-      <c r="H110" s="67"/>
-      <c r="I110" s="67"/>
-      <c r="J110" s="67"/>
-      <c r="K110" s="67"/>
-      <c r="L110" s="67"/>
-      <c r="M110" s="67"/>
-      <c r="N110" s="67"/>
-      <c r="O110" s="67"/>
-      <c r="P110" s="67"/>
-      <c r="Q110" s="67"/>
-      <c r="R110" s="67"/>
-      <c r="S110" s="67"/>
-      <c r="T110" s="67"/>
-      <c r="U110" s="67"/>
-      <c r="V110" s="67"/>
-      <c r="W110" s="67"/>
-      <c r="X110" s="67"/>
-      <c r="Y110" s="67"/>
-      <c r="Z110" s="67"/>
-      <c r="AA110" s="67"/>
-      <c r="AB110" s="67"/>
-      <c r="AC110" s="67"/>
-      <c r="AD110" s="67"/>
-      <c r="AE110" s="67"/>
-      <c r="AF110" s="67"/>
-      <c r="AG110" s="67"/>
-      <c r="AH110" s="67"/>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="C110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="D110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="E110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="F110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="G110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="H110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="I110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="J110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="K110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="L110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="M110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="N110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="O110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="P110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="Q110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="R110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="S110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="T110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="U110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="V110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="W110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="X110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="Y110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="Z110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="AA110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="AB110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="AC110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="AD110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="AE110" s="67" t="s">
+        <v>784</v>
+      </c>
+      <c r="AF110" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="AG110" s="67" t="s">
+        <v>783</v>
+      </c>
+      <c r="AH110" s="67" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="67"/>
-      <c r="B111" s="69" t="s">
+      <c r="B111" s="67"/>
+      <c r="C111" s="67"/>
+      <c r="D111" s="68" t="s">
         <v>785</v>
       </c>
-      <c r="C111" s="69"/>
-      <c r="D111" s="69"/>
-      <c r="E111" s="69" t="s">
-        <v>786</v>
-      </c>
-      <c r="F111" s="69"/>
-      <c r="G111" s="69"/>
-      <c r="H111" s="69" t="s">
-        <v>787</v>
-      </c>
-      <c r="I111" s="69"/>
-      <c r="J111" s="69"/>
-      <c r="K111" s="69" t="s">
-        <v>788</v>
-      </c>
-      <c r="L111" s="69"/>
-      <c r="M111" s="69"/>
-      <c r="N111" s="69" t="s">
-        <v>789</v>
-      </c>
-      <c r="O111" s="69"/>
-      <c r="P111" s="69"/>
-      <c r="Q111" s="69" t="s">
-        <v>790</v>
-      </c>
-      <c r="R111" s="69"/>
-      <c r="S111" s="69"/>
-      <c r="T111" s="69" t="s">
-        <v>791</v>
-      </c>
-      <c r="U111" s="69"/>
-      <c r="V111" s="69"/>
-      <c r="W111" s="69" t="s">
-        <v>792</v>
-      </c>
-      <c r="X111" s="69"/>
-      <c r="Y111" s="69"/>
-      <c r="Z111" s="69" t="s">
-        <v>793</v>
-      </c>
-      <c r="AA111" s="69"/>
-      <c r="AB111" s="69"/>
-      <c r="AC111" s="69" t="s">
-        <v>794</v>
-      </c>
-      <c r="AD111" s="69"/>
-      <c r="AE111" s="69"/>
-      <c r="AF111" s="69" t="s">
-        <v>795</v>
-      </c>
-      <c r="AG111" s="69"/>
-      <c r="AH111" s="69"/>
+      <c r="E111" s="67"/>
+      <c r="F111" s="67"/>
+      <c r="G111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="H111" s="67"/>
+      <c r="I111" s="67"/>
+      <c r="J111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="K111" s="67"/>
+      <c r="L111" s="67"/>
+      <c r="M111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="N111" s="67"/>
+      <c r="O111" s="67"/>
+      <c r="P111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="Q111" s="67"/>
+      <c r="R111" s="67"/>
+      <c r="S111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="T111" s="67"/>
+      <c r="U111" s="67"/>
+      <c r="V111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="W111" s="67"/>
+      <c r="X111" s="67"/>
+      <c r="Y111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="Z111" s="67"/>
+      <c r="AA111" s="67"/>
+      <c r="AB111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="AC111" s="67"/>
+      <c r="AD111" s="67"/>
+      <c r="AE111" s="68" t="s">
+        <v>785</v>
+      </c>
+      <c r="AF111" s="67"/>
+      <c r="AG111" s="67"/>
+      <c r="AH111" s="68" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="67"/>
@@ -18014,39 +17945,61 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="67"/>
-      <c r="B113" s="67"/>
-      <c r="C113" s="67"/>
-      <c r="D113" s="67"/>
-      <c r="E113" s="67"/>
-      <c r="F113" s="67"/>
-      <c r="G113" s="67"/>
-      <c r="H113" s="67"/>
-      <c r="I113" s="67"/>
-      <c r="J113" s="67"/>
-      <c r="K113" s="67"/>
-      <c r="L113" s="67"/>
-      <c r="M113" s="67"/>
-      <c r="N113" s="67"/>
-      <c r="O113" s="67"/>
-      <c r="P113" s="67"/>
-      <c r="Q113" s="67"/>
-      <c r="R113" s="67"/>
-      <c r="S113" s="67"/>
-      <c r="T113" s="67"/>
-      <c r="U113" s="67"/>
-      <c r="V113" s="67"/>
-      <c r="W113" s="67"/>
-      <c r="X113" s="67"/>
-      <c r="Y113" s="67"/>
-      <c r="Z113" s="67"/>
-      <c r="AA113" s="67"/>
-      <c r="AB113" s="67"/>
-      <c r="AC113" s="67"/>
-      <c r="AD113" s="67"/>
-      <c r="AE113" s="67"/>
-      <c r="AF113" s="67"/>
-      <c r="AG113" s="67"/>
-      <c r="AH113" s="67"/>
+      <c r="B113" s="69" t="s">
+        <v>786</v>
+      </c>
+      <c r="C113" s="69"/>
+      <c r="D113" s="69"/>
+      <c r="E113" s="69" t="s">
+        <v>787</v>
+      </c>
+      <c r="F113" s="69"/>
+      <c r="G113" s="69"/>
+      <c r="H113" s="69" t="s">
+        <v>788</v>
+      </c>
+      <c r="I113" s="69"/>
+      <c r="J113" s="69"/>
+      <c r="K113" s="69" t="s">
+        <v>789</v>
+      </c>
+      <c r="L113" s="69"/>
+      <c r="M113" s="69"/>
+      <c r="N113" s="69" t="s">
+        <v>790</v>
+      </c>
+      <c r="O113" s="69"/>
+      <c r="P113" s="69"/>
+      <c r="Q113" s="69" t="s">
+        <v>791</v>
+      </c>
+      <c r="R113" s="69"/>
+      <c r="S113" s="69"/>
+      <c r="T113" s="69" t="s">
+        <v>792</v>
+      </c>
+      <c r="U113" s="69"/>
+      <c r="V113" s="69"/>
+      <c r="W113" s="69" t="s">
+        <v>793</v>
+      </c>
+      <c r="X113" s="69"/>
+      <c r="Y113" s="69"/>
+      <c r="Z113" s="69" t="s">
+        <v>794</v>
+      </c>
+      <c r="AA113" s="69"/>
+      <c r="AB113" s="69"/>
+      <c r="AC113" s="69" t="s">
+        <v>795</v>
+      </c>
+      <c r="AD113" s="69"/>
+      <c r="AE113" s="69"/>
+      <c r="AF113" s="69" t="s">
+        <v>796</v>
+      </c>
+      <c r="AG113" s="69"/>
+      <c r="AH113" s="69"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="67"/>
@@ -18120,6 +18073,80 @@
       <c r="AG115" s="67"/>
       <c r="AH115" s="67"/>
     </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="67"/>
+      <c r="B116" s="67"/>
+      <c r="C116" s="67"/>
+      <c r="D116" s="67"/>
+      <c r="E116" s="67"/>
+      <c r="F116" s="67"/>
+      <c r="G116" s="67"/>
+      <c r="H116" s="67"/>
+      <c r="I116" s="67"/>
+      <c r="J116" s="67"/>
+      <c r="K116" s="67"/>
+      <c r="L116" s="67"/>
+      <c r="M116" s="67"/>
+      <c r="N116" s="67"/>
+      <c r="O116" s="67"/>
+      <c r="P116" s="67"/>
+      <c r="Q116" s="67"/>
+      <c r="R116" s="67"/>
+      <c r="S116" s="67"/>
+      <c r="T116" s="67"/>
+      <c r="U116" s="67"/>
+      <c r="V116" s="67"/>
+      <c r="W116" s="67"/>
+      <c r="X116" s="67"/>
+      <c r="Y116" s="67"/>
+      <c r="Z116" s="67"/>
+      <c r="AA116" s="67"/>
+      <c r="AB116" s="67"/>
+      <c r="AC116" s="67"/>
+      <c r="AD116" s="67"/>
+      <c r="AE116" s="67"/>
+      <c r="AF116" s="67"/>
+      <c r="AG116" s="67"/>
+      <c r="AH116" s="67"/>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="67"/>
+      <c r="B117" s="67"/>
+      <c r="C117" s="67"/>
+      <c r="D117" s="67"/>
+      <c r="E117" s="67"/>
+      <c r="F117" s="67"/>
+      <c r="G117" s="67"/>
+      <c r="H117" s="67"/>
+      <c r="I117" s="67"/>
+      <c r="J117" s="67"/>
+      <c r="K117" s="67"/>
+      <c r="L117" s="67"/>
+      <c r="M117" s="67"/>
+      <c r="N117" s="67"/>
+      <c r="O117" s="67"/>
+      <c r="P117" s="67"/>
+      <c r="Q117" s="67"/>
+      <c r="R117" s="67"/>
+      <c r="S117" s="67"/>
+      <c r="T117" s="67"/>
+      <c r="U117" s="67"/>
+      <c r="V117" s="67"/>
+      <c r="W117" s="67"/>
+      <c r="X117" s="67"/>
+      <c r="Y117" s="67"/>
+      <c r="Z117" s="67"/>
+      <c r="AA117" s="67"/>
+      <c r="AB117" s="67"/>
+      <c r="AC117" s="67"/>
+      <c r="AD117" s="67"/>
+      <c r="AE117" s="67"/>
+      <c r="AF117" s="67"/>
+      <c r="AG117" s="67"/>
+      <c r="AH117" s="67"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="22">
     <mergeCell ref="B1:D1"/>
@@ -18133,24 +18160,24 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="E111:G111"/>
-    <mergeCell ref="H111:J111"/>
-    <mergeCell ref="K111:M111"/>
-    <mergeCell ref="N111:P111"/>
-    <mergeCell ref="Q111:S111"/>
-    <mergeCell ref="T111:V111"/>
-    <mergeCell ref="W111:Y111"/>
-    <mergeCell ref="Z111:AB111"/>
-    <mergeCell ref="AC111:AE111"/>
-    <mergeCell ref="AF111:AH111"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="E113:G113"/>
+    <mergeCell ref="H113:J113"/>
+    <mergeCell ref="K113:M113"/>
+    <mergeCell ref="N113:P113"/>
+    <mergeCell ref="Q113:S113"/>
+    <mergeCell ref="T113:V113"/>
+    <mergeCell ref="W113:Y113"/>
+    <mergeCell ref="Z113:AB113"/>
+    <mergeCell ref="AC113:AE113"/>
+    <mergeCell ref="AF113:AH113"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="ISO 639-1 &gt;&gt;&#10;https://en.wikipedia.org/wiki/List_of_ISO_639-1_codes"/>
-    <hyperlink ref="B111" r:id="rId2" display="https://www.branah.com/english"/>
-    <hyperlink ref="N111" r:id="rId3" display="https://www.branah.com/portuguese"/>
-    <hyperlink ref="Q111" r:id="rId4" display="https://www.branah.com/italian"/>
-    <hyperlink ref="AF111" r:id="rId5" display="https://www.branah.com/greek"/>
+    <hyperlink ref="B113" r:id="rId2" display="https://www.branah.com/english"/>
+    <hyperlink ref="N113" r:id="rId3" display="https://www.branah.com/portuguese"/>
+    <hyperlink ref="Q113" r:id="rId4" display="https://www.branah.com/italian"/>
+    <hyperlink ref="AF113" r:id="rId5" display="https://www.branah.com/greek"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added Inl. Key for quick access
</commit_message>
<xml_diff>
--- a/keyboards/handwired/polykybd/split72/keymaps/default/lang/lang_lut.xlsx
+++ b/keyboards/handwired/polykybd/split72/keymaps/default/lang/lang_lut.xlsx
@@ -2984,7 +2984,7 @@
       <selection pane="topLeft" activeCell="D367" activeCellId="0" sqref="D367"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.74"/>
@@ -12354,16 +12354,16 @@
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
-      <selection pane="bottomRight" activeCell="J67" activeCellId="0" sqref="J67"/>
+      <selection pane="bottomLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
+      <selection pane="bottomRight" activeCell="B94" activeCellId="0" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="21.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="14" width="16.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="15" width="16.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="16" width="16.9"/>

</xml_diff>

<commit_message>
Added symbols, refactored ee access
</commit_message>
<xml_diff>
--- a/keyboards/handwired/polykybd/split72/keymaps/default/lang/lang_lut.xlsx
+++ b/keyboards/handwired/polykybd/split72/keymaps/default/lang/lang_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="named_glyphs" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="809">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -1837,6 +1837,42 @@
   </si>
   <si>
     <t xml:space="preserve">e5B6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE_FAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5B7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE_CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5B8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE_DOCUMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5B9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE_MIXED_DOCUMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5Ba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE_IMAGE_DOCUMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5Bb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE_IMAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5bc</t>
   </si>
   <si>
     <t xml:space="preserve">CLIPBOARD_PASTE</t>
@@ -2978,13 +3014,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G393"/>
+  <dimension ref="A1:G399"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A342" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D367" activeCellId="0" sqref="D367"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A357" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H375" activeCellId="0" sqref="H375"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.74"/>
@@ -12082,24 +12118,24 @@
       <c r="A379" s="0" t="s">
         <v>605</v>
       </c>
-      <c r="B379" s="9" t="s">
+      <c r="B379" s="12" t="s">
         <v>606</v>
       </c>
       <c r="C379" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B379)</f>
-        <v>58826</v>
+        <v>58807</v>
       </c>
       <c r="D379" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C379,4)</f>
-        <v>E5CA</v>
+        <v>E5B7</v>
       </c>
       <c r="E379" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C379)</f>
-        <v></v>
+        <v></v>
       </c>
       <c r="F379" s="0" t="n">
         <f aca="false">C379-C378</f>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G379" s="11"/>
     </row>
@@ -12107,24 +12143,24 @@
       <c r="A380" s="0" t="s">
         <v>607</v>
       </c>
-      <c r="B380" s="9" t="s">
+      <c r="B380" s="1" t="s">
         <v>608</v>
       </c>
       <c r="C380" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B380)</f>
-        <v>58837</v>
+        <v>58808</v>
       </c>
       <c r="D380" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C380,4)</f>
-        <v>E5D5</v>
+        <v>E5B8</v>
       </c>
       <c r="E380" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C380)</f>
-        <v></v>
+        <v></v>
       </c>
       <c r="F380" s="0" t="n">
         <f aca="false">C380-C379</f>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G380" s="11"/>
     </row>
@@ -12132,20 +12168,20 @@
       <c r="A381" s="0" t="s">
         <v>609</v>
       </c>
-      <c r="B381" s="1" t="s">
+      <c r="B381" s="12" t="s">
         <v>610</v>
       </c>
       <c r="C381" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B381)</f>
-        <v>58838</v>
+        <v>58809</v>
       </c>
       <c r="D381" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C381,4)</f>
-        <v>E5D6</v>
+        <v>E5B9</v>
       </c>
       <c r="E381" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C381)</f>
-        <v></v>
+        <v></v>
       </c>
       <c r="F381" s="0" t="n">
         <f aca="false">C381-C380</f>
@@ -12157,20 +12193,20 @@
       <c r="A382" s="0" t="s">
         <v>611</v>
       </c>
-      <c r="B382" s="9" t="s">
+      <c r="B382" s="1" t="s">
         <v>612</v>
       </c>
       <c r="C382" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B382)</f>
-        <v>58839</v>
+        <v>58810</v>
       </c>
       <c r="D382" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C382,4)</f>
-        <v>E5D7</v>
+        <v>E5BA</v>
       </c>
       <c r="E382" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C382)</f>
-        <v></v>
+        <v></v>
       </c>
       <c r="F382" s="0" t="n">
         <f aca="false">C382-C381</f>
@@ -12182,20 +12218,20 @@
       <c r="A383" s="0" t="s">
         <v>613</v>
       </c>
-      <c r="B383" s="1" t="s">
+      <c r="B383" s="12" t="s">
         <v>614</v>
       </c>
       <c r="C383" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B383)</f>
-        <v>58840</v>
+        <v>58811</v>
       </c>
       <c r="D383" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C383,4)</f>
-        <v>E5D8</v>
+        <v>E5BB</v>
       </c>
       <c r="E383" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C383)</f>
-        <v></v>
+        <v></v>
       </c>
       <c r="F383" s="0" t="n">
         <f aca="false">C383-C382</f>
@@ -12207,20 +12243,20 @@
       <c r="A384" s="0" t="s">
         <v>615</v>
       </c>
-      <c r="B384" s="9" t="s">
+      <c r="B384" s="1" t="s">
         <v>616</v>
       </c>
       <c r="C384" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B384)</f>
-        <v>58841</v>
+        <v>58812</v>
       </c>
       <c r="D384" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C384,4)</f>
-        <v>E5D9</v>
+        <v>E5BC</v>
       </c>
       <c r="E384" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C384)</f>
-        <v></v>
+        <v></v>
       </c>
       <c r="F384" s="0" t="n">
         <f aca="false">C384-C383</f>
@@ -12232,24 +12268,24 @@
       <c r="A385" s="0" t="s">
         <v>617</v>
       </c>
-      <c r="B385" s="1" t="s">
+      <c r="B385" s="9" t="s">
         <v>618</v>
       </c>
       <c r="C385" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B385)</f>
-        <v>58842</v>
+        <v>58826</v>
       </c>
       <c r="D385" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C385,4)</f>
-        <v>E5DA</v>
+        <v>E5CA</v>
       </c>
       <c r="E385" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C385)</f>
-        <v></v>
+        <v></v>
       </c>
       <c r="F385" s="0" t="n">
         <f aca="false">C385-C384</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G385" s="11"/>
     </row>
@@ -12262,19 +12298,19 @@
       </c>
       <c r="C386" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B386)</f>
-        <v>58843</v>
+        <v>58837</v>
       </c>
       <c r="D386" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C386,4)</f>
-        <v>E5DB</v>
+        <v>E5D5</v>
       </c>
       <c r="E386" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C386)</f>
-        <v></v>
+        <v></v>
       </c>
       <c r="F386" s="0" t="n">
         <f aca="false">C386-C385</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G386" s="11"/>
     </row>
@@ -12287,54 +12323,204 @@
       </c>
       <c r="C387" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B387)</f>
-        <v>65269</v>
+        <v>58838</v>
       </c>
       <c r="D387" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C387,4)</f>
-        <v>FEF5</v>
+        <v>E5D6</v>
       </c>
       <c r="E387" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C387)</f>
-        <v>ﻵ</v>
+        <v></v>
       </c>
       <c r="F387" s="0" t="n">
         <f aca="false">C387-C386</f>
-        <v>6426</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G387" s="11"/>
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="s">
         <v>623</v>
       </c>
-      <c r="B388" s="1" t="s">
+      <c r="B388" s="9" t="s">
         <v>624</v>
       </c>
       <c r="C388" s="0" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B388)</f>
-        <v>65275</v>
+        <v>58839</v>
       </c>
       <c r="D388" s="6" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C388,4)</f>
-        <v>FEFB</v>
+        <v>E5D7</v>
       </c>
       <c r="E388" s="7" t="str">
         <f aca="false">_xlfn.UNICHAR(C388)</f>
-        <v>ﻻ</v>
+        <v></v>
       </c>
       <c r="F388" s="0" t="n">
         <f aca="false">C388-C387</f>
+        <v>1</v>
+      </c>
+      <c r="G388" s="11"/>
+    </row>
+    <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="C389" s="0" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B389)</f>
+        <v>58840</v>
+      </c>
+      <c r="D389" s="6" t="str">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C389,4)</f>
+        <v>E5D8</v>
+      </c>
+      <c r="E389" s="7" t="str">
+        <f aca="false">_xlfn.UNICHAR(C389)</f>
+        <v></v>
+      </c>
+      <c r="F389" s="0" t="n">
+        <f aca="false">C389-C388</f>
+        <v>1</v>
+      </c>
+      <c r="G389" s="11"/>
+    </row>
+    <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A390" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="B390" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="C390" s="0" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B390)</f>
+        <v>58841</v>
+      </c>
+      <c r="D390" s="6" t="str">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C390,4)</f>
+        <v>E5D9</v>
+      </c>
+      <c r="E390" s="7" t="str">
+        <f aca="false">_xlfn.UNICHAR(C390)</f>
+        <v></v>
+      </c>
+      <c r="F390" s="0" t="n">
+        <f aca="false">C390-C389</f>
+        <v>1</v>
+      </c>
+      <c r="G390" s="11"/>
+    </row>
+    <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="s">
+        <v>629</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="C391" s="0" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B391)</f>
+        <v>58842</v>
+      </c>
+      <c r="D391" s="6" t="str">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C391,4)</f>
+        <v>E5DA</v>
+      </c>
+      <c r="E391" s="7" t="str">
+        <f aca="false">_xlfn.UNICHAR(C391)</f>
+        <v></v>
+      </c>
+      <c r="F391" s="0" t="n">
+        <f aca="false">C391-C390</f>
+        <v>1</v>
+      </c>
+      <c r="G391" s="11"/>
+    </row>
+    <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="0" t="s">
+        <v>631</v>
+      </c>
+      <c r="B392" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="C392" s="0" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B392)</f>
+        <v>58843</v>
+      </c>
+      <c r="D392" s="6" t="str">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C392,4)</f>
+        <v>E5DB</v>
+      </c>
+      <c r="E392" s="7" t="str">
+        <f aca="false">_xlfn.UNICHAR(C392)</f>
+        <v></v>
+      </c>
+      <c r="F392" s="0" t="n">
+        <f aca="false">C392-C391</f>
+        <v>1</v>
+      </c>
+      <c r="G392" s="11"/>
+    </row>
+    <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A393" s="0" t="s">
+        <v>633</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="C393" s="0" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B393)</f>
+        <v>65269</v>
+      </c>
+      <c r="D393" s="6" t="str">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C393,4)</f>
+        <v>FEF5</v>
+      </c>
+      <c r="E393" s="7" t="str">
+        <f aca="false">_xlfn.UNICHAR(C393)</f>
+        <v>ﻵ</v>
+      </c>
+      <c r="F393" s="0" t="n">
+        <f aca="false">C393-C392</f>
+        <v>6426</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A394" s="0" t="s">
+        <v>635</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="C394" s="0" t="n">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getHex2Dec(B394)</f>
+        <v>65275</v>
+      </c>
+      <c r="D394" s="6" t="str">
+        <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C394,4)</f>
+        <v>FEFB</v>
+      </c>
+      <c r="E394" s="7" t="str">
+        <f aca="false">_xlfn.UNICHAR(C394)</f>
+        <v>ﻻ</v>
+      </c>
+      <c r="F394" s="0" t="n">
+        <f aca="false">C394-C393</f>
         <v>6</v>
       </c>
     </row>
-    <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B389" s="0"/>
-    </row>
-    <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B393" s="10"/>
+    <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B395" s="0"/>
+    </row>
+    <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B399" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G363:G386"/>
+    <mergeCell ref="G363:G392"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -12353,7 +12539,7 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -12363,7 +12549,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="14" width="16.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="15" width="16.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="16" width="16.9"/>
@@ -12380,85 +12566,85 @@
   <sheetData>
     <row r="1" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>625</v>
+        <v>637</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>626</v>
+        <v>638</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
       <c r="E1" s="28" t="s">
-        <v>627</v>
+        <v>639</v>
       </c>
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
       <c r="H1" s="29" t="s">
-        <v>628</v>
+        <v>640</v>
       </c>
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
       <c r="K1" s="30" t="s">
-        <v>629</v>
+        <v>641</v>
       </c>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="31" t="s">
-        <v>630</v>
+        <v>642</v>
       </c>
       <c r="O1" s="31"/>
       <c r="P1" s="31"/>
       <c r="Q1" s="32" t="s">
-        <v>631</v>
+        <v>643</v>
       </c>
       <c r="R1" s="32"/>
       <c r="S1" s="32"/>
       <c r="T1" s="33" t="s">
-        <v>632</v>
+        <v>644</v>
       </c>
       <c r="U1" s="33"/>
       <c r="V1" s="33"/>
       <c r="W1" s="34" t="s">
-        <v>633</v>
+        <v>645</v>
       </c>
       <c r="X1" s="34"/>
       <c r="Y1" s="34"/>
       <c r="Z1" s="35" t="s">
-        <v>634</v>
+        <v>646</v>
       </c>
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
       <c r="AC1" s="36" t="s">
-        <v>635</v>
+        <v>647</v>
       </c>
       <c r="AD1" s="36"/>
       <c r="AE1" s="36"/>
       <c r="AF1" s="37" t="s">
-        <v>636</v>
+        <v>648</v>
       </c>
       <c r="AG1" s="37"/>
       <c r="AH1" s="37"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>637</v>
+        <v>649</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>638</v>
+        <v>650</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>639</v>
+        <v>651</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>640</v>
+        <v>652</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>641</v>
+        <v>653</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>638</v>
+        <v>650</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>639</v>
+        <v>651</v>
       </c>
       <c r="W2" s="21" t="s">
         <v>370</v>
@@ -12524,13 +12710,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>642</v>
+        <v>654</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>643</v>
+        <v>655</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>644</v>
+        <v>656</v>
       </c>
       <c r="W4" s="21" t="s">
         <v>402</v>
@@ -12539,10 +12725,10 @@
         <v>463</v>
       </c>
       <c r="AC4" s="23" t="s">
-        <v>623</v>
+        <v>635</v>
       </c>
       <c r="AD4" s="23" t="s">
-        <v>621</v>
+        <v>633</v>
       </c>
       <c r="AF4" s="24" t="s">
         <v>230</v>
@@ -12589,13 +12775,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>645</v>
+        <v>657</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>646</v>
+        <v>658</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>647</v>
+        <v>659</v>
       </c>
       <c r="W6" s="21" t="s">
         <v>382</v>
@@ -12661,13 +12847,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>648</v>
+        <v>660</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>649</v>
+        <v>661</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>650</v>
+        <v>662</v>
       </c>
       <c r="W8" s="21" t="s">
         <v>376</v>
@@ -12679,7 +12865,7 @@
         <v>336</v>
       </c>
       <c r="AD8" s="23" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="AE8" s="23" t="s">
         <v>336</v>
@@ -12729,49 +12915,49 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>652</v>
+        <v>664</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="T10" s="20" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="U10" s="20" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="W10" s="21" t="s">
         <v>367</v>
@@ -12789,7 +12975,7 @@
         <v>294</v>
       </c>
       <c r="AD10" s="52" t="s">
-        <v>655</v>
+        <v>667</v>
       </c>
       <c r="AE10" s="23" t="s">
         <v>294</v>
@@ -12867,13 +13053,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>656</v>
+        <v>668</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>657</v>
+        <v>669</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>658</v>
+        <v>670</v>
       </c>
       <c r="W12" s="21" t="s">
         <v>369</v>
@@ -12885,7 +13071,7 @@
         <v>290</v>
       </c>
       <c r="AD12" s="23" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="AE12" s="23" t="s">
         <v>290</v>
@@ -12935,13 +13121,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>661</v>
+        <v>673</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>662</v>
+        <v>674</v>
       </c>
       <c r="W14" s="21" t="s">
         <v>388</v>
@@ -12997,13 +13183,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>663</v>
+        <v>675</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>664</v>
+        <v>676</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>665</v>
+        <v>677</v>
       </c>
       <c r="W16" s="21" t="s">
         <v>397</v>
@@ -13065,19 +13251,19 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>666</v>
+        <v>678</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>667</v>
+        <v>679</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>668</v>
+        <v>680</v>
       </c>
       <c r="T18" s="20" t="s">
         <v>168</v>
       </c>
       <c r="U18" s="20" t="s">
-        <v>668</v>
+        <v>680</v>
       </c>
       <c r="W18" s="21" t="s">
         <v>391</v>
@@ -13122,10 +13308,10 @@
       <c r="R19" s="44"/>
       <c r="S19" s="44"/>
       <c r="T19" s="54" t="s">
-        <v>667</v>
+        <v>679</v>
       </c>
       <c r="U19" s="46" t="s">
-        <v>667</v>
+        <v>679</v>
       </c>
       <c r="V19" s="46"/>
       <c r="W19" s="47"/>
@@ -13143,13 +13329,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>669</v>
+        <v>681</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>670</v>
+        <v>682</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>671</v>
+        <v>683</v>
       </c>
       <c r="W20" s="21" t="s">
         <v>393</v>
@@ -13211,13 +13397,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>672</v>
+        <v>684</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>673</v>
+        <v>685</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>674</v>
+        <v>686</v>
       </c>
       <c r="W22" s="21" t="s">
         <v>389</v>
@@ -13279,13 +13465,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>675</v>
+        <v>687</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>676</v>
+        <v>688</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>677</v>
+        <v>689</v>
       </c>
       <c r="W24" s="21" t="s">
         <v>404</v>
@@ -13297,7 +13483,7 @@
         <v>331</v>
       </c>
       <c r="AD24" s="23" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="AE24" s="23" t="s">
         <v>331</v>
@@ -13347,25 +13533,25 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>679</v>
+        <v>691</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>680</v>
+        <v>692</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>681</v>
+        <v>693</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>680</v>
+        <v>692</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>681</v>
+        <v>693</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>682</v>
+        <v>694</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="W26" s="21" t="s">
         <v>403</v>
@@ -13431,13 +13617,13 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="s">
-        <v>684</v>
+        <v>696</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>685</v>
+        <v>697</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>686</v>
+        <v>698</v>
       </c>
       <c r="W28" s="21" t="s">
         <v>400</v>
@@ -13499,13 +13685,13 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
-        <v>687</v>
+        <v>699</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>688</v>
+        <v>700</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>689</v>
+        <v>701</v>
       </c>
       <c r="W30" s="21" t="s">
         <v>390</v>
@@ -13570,13 +13756,13 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="s">
-        <v>690</v>
+        <v>702</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>691</v>
+        <v>703</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>692</v>
+        <v>704</v>
       </c>
       <c r="W32" s="21" t="s">
         <v>394</v>
@@ -13641,31 +13827,31 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="s">
-        <v>693</v>
+        <v>705</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>640</v>
+        <v>652</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>641</v>
+        <v>653</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>640</v>
+        <v>652</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>641</v>
+        <v>653</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>638</v>
+        <v>650</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>639</v>
+        <v>651</v>
       </c>
       <c r="T34" s="20" t="s">
-        <v>640</v>
+        <v>652</v>
       </c>
       <c r="U34" s="20" t="s">
-        <v>641</v>
+        <v>653</v>
       </c>
       <c r="W34" s="21" t="s">
         <v>371</v>
@@ -13680,19 +13866,19 @@
         <v>310</v>
       </c>
       <c r="AD34" s="52" t="s">
-        <v>694</v>
+        <v>706</v>
       </c>
       <c r="AE34" s="23" t="s">
         <v>310</v>
       </c>
       <c r="AF34" s="24" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="AG34" s="53" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="AH34" s="24" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
     </row>
     <row r="35" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13701,10 +13887,10 @@
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>
       <c r="E35" s="40" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="F35" s="40" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="G35" s="40"/>
       <c r="H35" s="41"/>
@@ -13720,10 +13906,10 @@
       <c r="R35" s="44"/>
       <c r="S35" s="44"/>
       <c r="T35" s="46" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="U35" s="46" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="V35" s="46"/>
       <c r="W35" s="47"/>
@@ -13741,13 +13927,13 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="s">
-        <v>698</v>
+        <v>710</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>699</v>
+        <v>711</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>700</v>
+        <v>712</v>
       </c>
       <c r="W36" s="21" t="s">
         <v>364</v>
@@ -13762,7 +13948,7 @@
         <v>328</v>
       </c>
       <c r="AD36" s="52" t="s">
-        <v>701</v>
+        <v>713</v>
       </c>
       <c r="AE36" s="23" t="s">
         <v>328</v>
@@ -13826,13 +14012,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="s">
-        <v>702</v>
+        <v>714</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>703</v>
+        <v>715</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="W38" s="21" t="s">
         <v>366</v>
@@ -13888,13 +14074,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="s">
-        <v>705</v>
+        <v>717</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>706</v>
+        <v>718</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>707</v>
+        <v>719</v>
       </c>
       <c r="W40" s="21" t="s">
         <v>373</v>
@@ -13953,13 +14139,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13" t="s">
-        <v>708</v>
+        <v>720</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>709</v>
+        <v>721</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>710</v>
+        <v>722</v>
       </c>
       <c r="W42" s="21" t="s">
         <v>395</v>
@@ -14021,13 +14207,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13" t="s">
-        <v>711</v>
+        <v>723</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>712</v>
+        <v>724</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>713</v>
+        <v>725</v>
       </c>
       <c r="W44" s="21" t="s">
         <v>387</v>
@@ -14089,19 +14275,19 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="s">
-        <v>714</v>
+        <v>726</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>715</v>
+        <v>727</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>717</v>
+        <v>729</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="W46" s="21" t="s">
         <v>378</v>
@@ -14116,7 +14302,7 @@
         <v>309</v>
       </c>
       <c r="AD46" s="52" t="s">
-        <v>719</v>
+        <v>731</v>
       </c>
       <c r="AE46" s="23" t="s">
         <v>309</v>
@@ -14169,13 +14355,13 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="s">
-        <v>720</v>
+        <v>732</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>721</v>
+        <v>733</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>722</v>
+        <v>734</v>
       </c>
       <c r="W48" s="21" t="s">
         <v>386</v>
@@ -14187,7 +14373,7 @@
         <v>283</v>
       </c>
       <c r="AD48" s="52" t="s">
-        <v>723</v>
+        <v>735</v>
       </c>
       <c r="AE48" s="23" t="s">
         <v>283</v>
@@ -14237,19 +14423,19 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="13" t="s">
-        <v>724</v>
+        <v>736</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>725</v>
+        <v>737</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>717</v>
+        <v>729</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="W50" s="21" t="s">
         <v>398</v>
@@ -14315,25 +14501,25 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="13" t="s">
+        <v>739</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>729</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>730</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>738</v>
+      </c>
+      <c r="H52" s="16" t="s">
         <v>727</v>
       </c>
-      <c r="B52" s="14" t="s">
-        <v>717</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>718</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>725</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>726</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>715</v>
-      </c>
       <c r="I52" s="16" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
       <c r="W52" s="21" t="s">
         <v>384</v>
@@ -14348,7 +14534,7 @@
         <v>288</v>
       </c>
       <c r="AD52" s="23" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="AE52" s="23" t="s">
         <v>288</v>
@@ -14395,13 +14581,13 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="13" t="s">
-        <v>729</v>
+        <v>741</v>
       </c>
       <c r="B54" s="14" t="n">
         <v>1</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="D54" s="14" t="n">
         <v>1</v>
@@ -14410,10 +14596,10 @@
         <v>1</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="I54" s="16" t="n">
         <v>1</v>
@@ -14422,7 +14608,7 @@
         <v>1</v>
       </c>
       <c r="L54" s="17" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="M54" s="17" t="n">
         <v>1</v>
@@ -14431,7 +14617,7 @@
         <v>1</v>
       </c>
       <c r="U54" s="20" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="V54" s="20" t="n">
         <v>1</v>
@@ -14443,7 +14629,7 @@
         <v>1</v>
       </c>
       <c r="AD54" s="23" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="AE54" s="23" t="n">
         <v>1</v>
@@ -14452,7 +14638,7 @@
         <v>1</v>
       </c>
       <c r="AG54" s="24" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="AH54" s="24" t="n">
         <v>1</v>
@@ -14461,7 +14647,7 @@
     <row r="55" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="38"/>
       <c r="B55" s="39" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="C55" s="39"/>
       <c r="D55" s="39"/>
@@ -14472,13 +14658,13 @@
       <c r="I55" s="41"/>
       <c r="J55" s="41"/>
       <c r="K55" s="42" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="L55" s="42" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="M55" s="42" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="N55" s="43"/>
       <c r="O55" s="43"/>
@@ -14487,13 +14673,13 @@
       <c r="R55" s="44"/>
       <c r="S55" s="44"/>
       <c r="T55" s="46" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="U55" s="46" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="V55" s="46" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="W55" s="47"/>
       <c r="X55" s="47"/>
@@ -14516,13 +14702,13 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="13" t="s">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="B56" s="14" t="n">
         <v>2</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="D56" s="14" t="n">
         <v>2</v>
@@ -14570,7 +14756,7 @@
         <v>2</v>
       </c>
       <c r="U56" s="20" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="V56" s="20" t="n">
         <v>2</v>
@@ -14582,7 +14768,7 @@
         <v>2</v>
       </c>
       <c r="AD56" s="23" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="AE56" s="23" t="n">
         <v>2</v>
@@ -14591,7 +14777,7 @@
         <v>2</v>
       </c>
       <c r="AG56" s="24" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="AH56" s="24" t="n">
         <v>2</v>
@@ -14600,7 +14786,7 @@
     <row r="57" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="38"/>
       <c r="B57" s="39" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="C57" s="39"/>
       <c r="D57" s="39"/>
@@ -14612,29 +14798,29 @@
       </c>
       <c r="G57" s="40"/>
       <c r="H57" s="41" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="I57" s="41" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="J57" s="41"/>
       <c r="K57" s="42" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="L57" s="42" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="M57" s="42" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="N57" s="43" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="O57" s="43" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="P57" s="43" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="Q57" s="44"/>
       <c r="R57" s="44"/>
@@ -14675,13 +14861,13 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="13" t="s">
-        <v>736</v>
+        <v>748</v>
       </c>
       <c r="B58" s="14" t="n">
         <v>3</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="D58" s="14" t="n">
         <v>3</v>
@@ -14711,7 +14897,7 @@
         <v>3</v>
       </c>
       <c r="O58" s="18" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="P58" s="18" t="n">
         <v>3</v>
@@ -14729,7 +14915,7 @@
         <v>3</v>
       </c>
       <c r="U58" s="20" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="V58" s="20" t="n">
         <v>3</v>
@@ -14744,7 +14930,7 @@
         <v>3</v>
       </c>
       <c r="AD58" s="23" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="AE58" s="23" t="n">
         <v>3</v>
@@ -14753,7 +14939,7 @@
         <v>3</v>
       </c>
       <c r="AG58" s="24" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="AH58" s="24" t="n">
         <v>3</v>
@@ -14762,7 +14948,7 @@
     <row r="59" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="38"/>
       <c r="B59" s="39" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="C59" s="39"/>
       <c r="D59" s="39"/>
@@ -14774,20 +14960,20 @@
       </c>
       <c r="G59" s="40"/>
       <c r="H59" s="41" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="I59" s="41" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="J59" s="41"/>
       <c r="K59" s="42" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="L59" s="42" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="M59" s="42" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="N59" s="43" t="s">
         <v>47</v>
@@ -14802,13 +14988,13 @@
       <c r="R59" s="44"/>
       <c r="S59" s="44"/>
       <c r="T59" s="46" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="U59" s="46" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="V59" s="46" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="W59" s="47"/>
       <c r="X59" s="47"/>
@@ -14829,7 +15015,7 @@
         <v>76</v>
       </c>
       <c r="AG59" s="24" t="s">
-        <v>739</v>
+        <v>751</v>
       </c>
       <c r="AH59" s="24" t="s">
         <v>76</v>
@@ -14837,13 +15023,13 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13" t="s">
-        <v>740</v>
+        <v>752</v>
       </c>
       <c r="B60" s="14" t="n">
         <v>4</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="D60" s="14" t="n">
         <v>4</v>
@@ -14852,10 +15038,10 @@
         <v>4</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="I60" s="16" t="n">
         <v>4</v>
@@ -14864,7 +15050,7 @@
         <v>4</v>
       </c>
       <c r="L60" s="17" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="M60" s="17" t="n">
         <v>4</v>
@@ -14873,7 +15059,7 @@
         <v>4</v>
       </c>
       <c r="O60" s="18" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="P60" s="18" t="n">
         <v>4</v>
@@ -14882,7 +15068,7 @@
         <v>4</v>
       </c>
       <c r="U60" s="20" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="V60" s="20" t="n">
         <v>4</v>
@@ -14897,7 +15083,7 @@
         <v>4</v>
       </c>
       <c r="AD60" s="23" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="AE60" s="23" t="n">
         <v>4</v>
@@ -14906,7 +15092,7 @@
         <v>4</v>
       </c>
       <c r="AG60" s="24" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="AH60" s="24" t="n">
         <v>4</v>
@@ -14915,7 +15101,7 @@
     <row r="61" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="38"/>
       <c r="B61" s="39" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="C61" s="39"/>
       <c r="D61" s="39"/>
@@ -14923,20 +15109,20 @@
       <c r="F61" s="40"/>
       <c r="G61" s="40"/>
       <c r="H61" s="41" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="I61" s="41" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="J61" s="41"/>
       <c r="K61" s="42" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="L61" s="42" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="M61" s="42" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="N61" s="43" t="s">
         <v>55</v>
@@ -14951,13 +15137,13 @@
       <c r="R61" s="44"/>
       <c r="S61" s="44"/>
       <c r="T61" s="46" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="U61" s="46" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="V61" s="46" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="W61" s="47"/>
       <c r="X61" s="47"/>
@@ -14986,13 +15172,13 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="13" t="s">
-        <v>744</v>
+        <v>756</v>
       </c>
       <c r="B62" s="14" t="n">
         <v>5</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="D62" s="14" t="n">
         <v>5</v>
@@ -15001,10 +15187,10 @@
         <v>5</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="I62" s="16" t="n">
         <v>5</v>
@@ -15013,7 +15199,7 @@
         <v>5</v>
       </c>
       <c r="L62" s="17" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="M62" s="17" t="n">
         <v>5</v>
@@ -15022,7 +15208,7 @@
         <v>5</v>
       </c>
       <c r="O62" s="18" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="P62" s="18" t="n">
         <v>5</v>
@@ -15031,7 +15217,7 @@
         <v>5</v>
       </c>
       <c r="U62" s="20" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="V62" s="20" t="n">
         <v>5</v>
@@ -15046,7 +15232,7 @@
         <v>5</v>
       </c>
       <c r="AD62" s="23" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="AE62" s="23" t="n">
         <v>5</v>
@@ -15055,7 +15241,7 @@
         <v>5</v>
       </c>
       <c r="AG62" s="24" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="AH62" s="24" t="n">
         <v>5</v>
@@ -15064,7 +15250,7 @@
     <row r="63" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="38"/>
       <c r="B63" s="39" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="C63" s="39"/>
       <c r="D63" s="39"/>
@@ -15072,10 +15258,10 @@
       <c r="F63" s="40"/>
       <c r="G63" s="40"/>
       <c r="H63" s="41" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="I63" s="41" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="J63" s="41"/>
       <c r="K63" s="42" t="s">
@@ -15135,13 +15321,13 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="13" t="s">
-        <v>747</v>
+        <v>759</v>
       </c>
       <c r="B64" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="D64" s="14" t="n">
         <v>6</v>
@@ -15150,10 +15336,10 @@
         <v>6</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="I64" s="16" t="n">
         <v>6</v>
@@ -15162,7 +15348,7 @@
         <v>6</v>
       </c>
       <c r="L64" s="17" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="M64" s="17" t="n">
         <v>6</v>
@@ -15171,7 +15357,7 @@
         <v>6</v>
       </c>
       <c r="O64" s="18" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="P64" s="18" t="n">
         <v>6</v>
@@ -15180,7 +15366,7 @@
         <v>6</v>
       </c>
       <c r="R64" s="19" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="S64" s="19" t="n">
         <v>6</v>
@@ -15189,7 +15375,7 @@
         <v>6</v>
       </c>
       <c r="U64" s="20" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="V64" s="20" t="n">
         <v>6</v>
@@ -15204,7 +15390,7 @@
         <v>6</v>
       </c>
       <c r="AD64" s="23" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="AE64" s="23" t="n">
         <v>6</v>
@@ -15213,7 +15399,7 @@
         <v>6</v>
       </c>
       <c r="AG64" s="24" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="AH64" s="24" t="n">
         <v>6</v>
@@ -15222,7 +15408,7 @@
     <row r="65" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="38"/>
       <c r="B65" s="39" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="C65" s="39"/>
       <c r="D65" s="39"/>
@@ -15230,10 +15416,10 @@
       <c r="F65" s="40"/>
       <c r="G65" s="40"/>
       <c r="H65" s="41" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="I65" s="41" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="J65" s="41"/>
       <c r="K65" s="42" t="s">
@@ -15281,13 +15467,13 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="13" t="s">
-        <v>749</v>
+        <v>761</v>
       </c>
       <c r="B66" s="14" t="n">
         <v>7</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="D66" s="14" t="n">
         <v>7</v>
@@ -15296,7 +15482,7 @@
         <v>7</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="H66" s="16" t="s">
         <v>136</v>
@@ -15308,7 +15494,7 @@
         <v>7</v>
       </c>
       <c r="L66" s="17" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="M66" s="17" t="n">
         <v>7</v>
@@ -15317,7 +15503,7 @@
         <v>7</v>
       </c>
       <c r="O66" s="18" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="P66" s="18" t="n">
         <v>7</v>
@@ -15326,7 +15512,7 @@
         <v>7</v>
       </c>
       <c r="R66" s="19" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="S66" s="19" t="n">
         <v>7</v>
@@ -15335,7 +15521,7 @@
         <v>7</v>
       </c>
       <c r="U66" s="20" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="V66" s="20" t="n">
         <v>7</v>
@@ -15350,7 +15536,7 @@
         <v>7</v>
       </c>
       <c r="AD66" s="23" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="AE66" s="23" t="n">
         <v>7</v>
@@ -15359,7 +15545,7 @@
         <v>7</v>
       </c>
       <c r="AG66" s="24" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="AH66" s="24" t="n">
         <v>7</v>
@@ -15368,15 +15554,15 @@
     <row r="67" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="38"/>
       <c r="B67" s="39" t="s">
-        <v>731</v>
+        <v>743</v>
       </c>
       <c r="C67" s="39"/>
       <c r="D67" s="39"/>
       <c r="E67" s="40" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="F67" s="40" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="G67" s="40"/>
       <c r="H67" s="16" t="s">
@@ -15390,25 +15576,25 @@
       <c r="L67" s="42"/>
       <c r="M67" s="42"/>
       <c r="N67" s="43" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="O67" s="43" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="P67" s="43" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="Q67" s="44"/>
       <c r="R67" s="44"/>
       <c r="S67" s="44"/>
       <c r="T67" s="46" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="U67" s="46" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="V67" s="46" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="W67" s="47"/>
       <c r="X67" s="47"/>
@@ -15431,13 +15617,13 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="13" t="s">
-        <v>750</v>
+        <v>762</v>
       </c>
       <c r="B68" s="14" t="n">
         <v>8</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="D68" s="14" t="n">
         <v>8</v>
@@ -15446,10 +15632,10 @@
         <v>8</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="I68" s="16" t="n">
         <v>8</v>
@@ -15458,7 +15644,7 @@
         <v>8</v>
       </c>
       <c r="L68" s="17" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="M68" s="17" t="n">
         <v>8</v>
@@ -15467,7 +15653,7 @@
         <v>8</v>
       </c>
       <c r="O68" s="18" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="P68" s="18" t="n">
         <v>8</v>
@@ -15476,7 +15662,7 @@
         <v>8</v>
       </c>
       <c r="R68" s="19" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="S68" s="19" t="n">
         <v>8</v>
@@ -15485,7 +15671,7 @@
         <v>8</v>
       </c>
       <c r="U68" s="20" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="V68" s="20" t="n">
         <v>8</v>
@@ -15500,7 +15686,7 @@
         <v>8</v>
       </c>
       <c r="AD68" s="23" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="AE68" s="23" t="n">
         <v>8</v>
@@ -15509,7 +15695,7 @@
         <v>8</v>
       </c>
       <c r="AG68" s="24" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="AH68" s="24" t="n">
         <v>8</v>
@@ -15518,15 +15704,15 @@
     <row r="69" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="38"/>
       <c r="B69" s="39" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="C69" s="39"/>
       <c r="D69" s="39"/>
       <c r="E69" s="40" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="F69" s="40" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="G69" s="40"/>
       <c r="H69" s="41" t="s">
@@ -15540,25 +15726,25 @@
       <c r="L69" s="42"/>
       <c r="M69" s="42"/>
       <c r="N69" s="43" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="O69" s="43" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="P69" s="43" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="Q69" s="44"/>
       <c r="R69" s="44"/>
       <c r="S69" s="44"/>
       <c r="T69" s="46" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="U69" s="46" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="V69" s="46" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="W69" s="47"/>
       <c r="X69" s="47"/>
@@ -15587,13 +15773,13 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="13" t="s">
-        <v>753</v>
+        <v>765</v>
       </c>
       <c r="B70" s="14" t="n">
         <v>9</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="D70" s="14" t="n">
         <v>9</v>
@@ -15602,7 +15788,7 @@
         <v>9</v>
       </c>
       <c r="F70" s="15" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="H70" s="57" t="s">
         <v>134</v>
@@ -15615,7 +15801,7 @@
         <v>9</v>
       </c>
       <c r="L70" s="17" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="M70" s="17" t="n">
         <v>9</v>
@@ -15624,7 +15810,7 @@
         <v>9</v>
       </c>
       <c r="O70" s="18" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="P70" s="18" t="n">
         <v>9</v>
@@ -15633,7 +15819,7 @@
         <v>9</v>
       </c>
       <c r="R70" s="19" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="S70" s="19" t="n">
         <v>9</v>
@@ -15642,7 +15828,7 @@
         <v>9</v>
       </c>
       <c r="U70" s="20" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="V70" s="20" t="n">
         <v>9</v>
@@ -15657,7 +15843,7 @@
         <v>9</v>
       </c>
       <c r="AD70" s="23" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="AE70" s="23" t="n">
         <v>9</v>
@@ -15666,7 +15852,7 @@
         <v>9</v>
       </c>
       <c r="AG70" s="24" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="AH70" s="24" t="n">
         <v>9</v>
@@ -15675,47 +15861,47 @@
     <row r="71" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="38"/>
       <c r="B71" s="39" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="C71" s="39"/>
       <c r="D71" s="39"/>
       <c r="E71" s="40" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="F71" s="40" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="G71" s="40"/>
       <c r="H71" s="41" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="I71" s="41" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="J71" s="41"/>
       <c r="K71" s="42"/>
       <c r="L71" s="42"/>
       <c r="M71" s="42"/>
       <c r="N71" s="43" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="O71" s="43" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="P71" s="43" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="Q71" s="44"/>
       <c r="R71" s="44"/>
       <c r="S71" s="44"/>
       <c r="T71" s="46" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="U71" s="46" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="V71" s="46" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="W71" s="47"/>
       <c r="X71" s="47"/>
@@ -15744,13 +15930,13 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="13" t="s">
-        <v>755</v>
+        <v>767</v>
       </c>
       <c r="B72" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="D72" s="14" t="s">
         <v>12</v>
@@ -15814,7 +16000,7 @@
         <v>12</v>
       </c>
       <c r="AD72" s="23" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="AE72" s="23" t="s">
         <v>12</v>
@@ -15823,7 +16009,7 @@
         <v>0</v>
       </c>
       <c r="AG72" s="24" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="AH72" s="24" t="n">
         <v>0</v>
@@ -15832,47 +16018,47 @@
     <row r="73" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="38"/>
       <c r="B73" s="39" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="C73" s="39"/>
       <c r="D73" s="39"/>
       <c r="E73" s="40" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="F73" s="40" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="G73" s="40"/>
       <c r="H73" s="41" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="I73" s="41" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="J73" s="41"/>
       <c r="K73" s="42"/>
       <c r="L73" s="42"/>
       <c r="M73" s="42"/>
       <c r="N73" s="43" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="O73" s="43" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="P73" s="43" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="Q73" s="44"/>
       <c r="R73" s="44"/>
       <c r="S73" s="44"/>
       <c r="T73" s="46" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="U73" s="46" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="V73" s="46" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="W73" s="47"/>
       <c r="X73" s="47"/>
@@ -15901,7 +16087,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="13" t="s">
-        <v>757</v>
+        <v>769</v>
       </c>
       <c r="B74" s="58" t="s">
         <v>431</v>
@@ -15945,10 +16131,10 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="13" t="s">
-        <v>758</v>
+        <v>770</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>759</v>
+        <v>771</v>
       </c>
     </row>
     <row r="77" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15989,7 +16175,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="13" t="s">
-        <v>760</v>
+        <v>772</v>
       </c>
       <c r="B78" s="14" t="s">
         <v>410</v>
@@ -16033,7 +16219,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="s">
-        <v>761</v>
+        <v>773</v>
       </c>
       <c r="B80" s="59" t="s">
         <v>425</v>
@@ -16077,7 +16263,7 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="13" t="s">
-        <v>762</v>
+        <v>774</v>
       </c>
       <c r="B82" s="14" t="s">
         <v>24</v>
@@ -16121,67 +16307,67 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="13" t="s">
-        <v>763</v>
+        <v>775</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="E84" s="15" t="s">
         <v>126</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>126</v>
       </c>
       <c r="H84" s="16" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="I84" s="57" t="s">
         <v>70</v>
       </c>
       <c r="K84" s="17" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="L84" s="17" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="M84" s="17" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="N84" s="18" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="O84" s="18" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="P84" s="18" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="Q84" s="19" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="R84" s="19" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="S84" s="19" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="T84" s="20" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="U84" s="20" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="V84" s="20" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="Z84" s="22" t="s">
         <v>516</v>
@@ -16190,19 +16376,19 @@
         <v>570</v>
       </c>
       <c r="AF84" s="24" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="AG84" s="24" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="AH84" s="24" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
     </row>
     <row r="85" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="38"/>
       <c r="B85" s="39" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="C85" s="39"/>
       <c r="D85" s="39"/>
@@ -16216,10 +16402,10 @@
         <v>16</v>
       </c>
       <c r="H85" s="41" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="I85" s="41" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="J85" s="41"/>
       <c r="K85" s="42"/>
@@ -16229,13 +16415,13 @@
       <c r="O85" s="43"/>
       <c r="P85" s="43"/>
       <c r="Q85" s="44" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="R85" s="44" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="S85" s="44" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="T85" s="46" t="s">
         <v>16</v>
@@ -16267,13 +16453,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="13" t="s">
-        <v>764</v>
+        <v>776</v>
       </c>
       <c r="B86" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="D86" s="14" t="s">
         <v>14</v>
@@ -16291,7 +16477,7 @@
         <v>14</v>
       </c>
       <c r="I86" s="16" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="K86" s="17" t="s">
         <v>45</v>
@@ -16321,13 +16507,13 @@
         <v>105</v>
       </c>
       <c r="T86" s="62" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="U86" s="62" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="V86" s="62" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="Z86" s="22" t="s">
         <v>512</v>
@@ -16336,7 +16522,7 @@
         <v>14</v>
       </c>
       <c r="AG86" s="24" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="AH86" s="24" t="s">
         <v>14</v>
@@ -16345,7 +16531,7 @@
     <row r="87" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="38"/>
       <c r="B87" s="39" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="C87" s="39"/>
       <c r="D87" s="39"/>
@@ -16353,10 +16539,10 @@
       <c r="F87" s="40"/>
       <c r="G87" s="40"/>
       <c r="H87" s="41" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="I87" s="41" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="J87" s="41"/>
       <c r="K87" s="42"/>
@@ -16375,13 +16561,13 @@
         <v>144</v>
       </c>
       <c r="T87" s="46" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="U87" s="46" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="V87" s="46" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="W87" s="47"/>
       <c r="X87" s="47"/>
@@ -16404,16 +16590,16 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="13" t="s">
-        <v>765</v>
+        <v>777</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="E88" s="15" t="s">
         <v>160</v>
@@ -16422,7 +16608,7 @@
         <v>124</v>
       </c>
       <c r="H88" s="16" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="I88" s="57" t="s">
         <v>57</v>
@@ -16431,19 +16617,19 @@
         <v>18</v>
       </c>
       <c r="L88" s="17" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="M88" s="17" t="s">
         <v>18</v>
       </c>
       <c r="N88" s="18" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="O88" s="18" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="P88" s="18" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="Q88" s="19" t="s">
         <v>136</v>
@@ -16470,25 +16656,25 @@
         <v>296</v>
       </c>
       <c r="AD88" s="23" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="AE88" s="23" t="s">
         <v>296</v>
       </c>
       <c r="AF88" s="24" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="AG88" s="24" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="AH88" s="24" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
     </row>
     <row r="89" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="38"/>
       <c r="B89" s="39" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="C89" s="39"/>
       <c r="D89" s="39"/>
@@ -16499,13 +16685,13 @@
       <c r="I89" s="41"/>
       <c r="J89" s="41"/>
       <c r="K89" s="42" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="L89" s="42" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="M89" s="42" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="N89" s="63" t="s">
         <v>57</v>
@@ -16517,19 +16703,19 @@
         <v>57</v>
       </c>
       <c r="Q89" s="64" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="R89" s="64" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="S89" s="64" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
       <c r="T89" s="45" t="s">
-        <v>766</v>
+        <v>778</v>
       </c>
       <c r="U89" s="45" t="s">
-        <v>766</v>
+        <v>778</v>
       </c>
       <c r="V89" s="45"/>
       <c r="W89" s="47"/>
@@ -16553,37 +16739,37 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="13" t="s">
-        <v>767</v>
+        <v>779</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="E90" s="15" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="F90" s="15" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="H90" s="16" t="s">
-        <v>741</v>
+        <v>753</v>
       </c>
       <c r="I90" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K90" s="17" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="L90" s="17" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="M90" s="17" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="N90" s="60" t="s">
         <v>78</v>
@@ -16595,13 +16781,13 @@
         <v>78</v>
       </c>
       <c r="Q90" s="61" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="R90" s="61" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="S90" s="61" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="T90" s="62" t="s">
         <v>160</v>
@@ -16620,33 +16806,33 @@
         <v>302</v>
       </c>
       <c r="AD90" s="23" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="AE90" s="23" t="s">
         <v>302</v>
       </c>
       <c r="AF90" s="24" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="AG90" s="24" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="AH90" s="24" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
     </row>
     <row r="91" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="38"/>
       <c r="B91" s="39" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="C91" s="39"/>
       <c r="D91" s="39"/>
       <c r="E91" s="40" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="F91" s="40" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="G91" s="40"/>
       <c r="H91" s="65" t="s">
@@ -16657,37 +16843,37 @@
       </c>
       <c r="J91" s="65"/>
       <c r="K91" s="42" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="L91" s="42" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="M91" s="42" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="N91" s="43" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="O91" s="43" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="P91" s="43" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="Q91" s="44" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="R91" s="44" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="S91" s="44" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="T91" s="46" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="U91" s="46" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="V91" s="46"/>
       <c r="W91" s="47"/>
@@ -16711,25 +16897,25 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="13" t="s">
-        <v>768</v>
+        <v>780</v>
       </c>
       <c r="B92" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="D92" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E92" s="15" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="F92" s="15" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="H92" s="16" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="I92" s="16" t="s">
         <v>80</v>
@@ -16741,13 +16927,13 @@
         <v>99</v>
       </c>
       <c r="N92" s="18" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="O92" s="18" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="P92" s="18" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="Q92" s="19" t="s">
         <v>156</v>
@@ -16759,10 +16945,10 @@
         <v>120</v>
       </c>
       <c r="T92" s="20" t="s">
-        <v>682</v>
+        <v>694</v>
       </c>
       <c r="U92" s="20" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="Z92" s="22" t="s">
         <v>526</v>
@@ -16771,7 +16957,7 @@
         <v>304</v>
       </c>
       <c r="AD92" s="52" t="s">
-        <v>769</v>
+        <v>781</v>
       </c>
       <c r="AE92" s="23" t="s">
         <v>304</v>
@@ -16780,7 +16966,7 @@
         <v>16</v>
       </c>
       <c r="AG92" s="53" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="AH92" s="24" t="s">
         <v>16</v>
@@ -16789,7 +16975,7 @@
     <row r="93" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="38"/>
       <c r="B93" s="39" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="C93" s="39"/>
       <c r="D93" s="39"/>
@@ -16800,10 +16986,10 @@
       <c r="I93" s="41"/>
       <c r="J93" s="41"/>
       <c r="K93" s="42" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="L93" s="42" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="M93" s="42"/>
       <c r="N93" s="43"/>
@@ -16846,33 +17032,33 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="13" t="s">
-        <v>770</v>
+        <v>782</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="E94" s="15" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="F94" s="15" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
     </row>
     <row r="95" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="38"/>
       <c r="B95" s="39" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="C95" s="39"/>
       <c r="D95" s="39"/>
       <c r="E95" s="40" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="F95" s="40"/>
       <c r="G95" s="40"/>
@@ -16906,16 +17092,16 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="13" t="s">
-        <v>771</v>
+        <v>783</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="E96" s="15" t="s">
         <v>152</v>
@@ -16924,10 +17110,10 @@
         <v>116</v>
       </c>
       <c r="H96" s="16" t="s">
-        <v>680</v>
+        <v>692</v>
       </c>
       <c r="I96" s="16" t="s">
-        <v>681</v>
+        <v>693</v>
       </c>
       <c r="K96" s="17" t="s">
         <v>146</v>
@@ -16963,7 +17149,7 @@
         <v>329</v>
       </c>
       <c r="AD96" s="23" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="AE96" s="23" t="s">
         <v>329</v>
@@ -16981,7 +17167,7 @@
     <row r="97" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="38"/>
       <c r="B97" s="39" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="C97" s="39"/>
       <c r="D97" s="39"/>
@@ -16998,13 +17184,13 @@
       <c r="O97" s="43"/>
       <c r="P97" s="43"/>
       <c r="Q97" s="44" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="R97" s="44" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="S97" s="44" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="T97" s="46" t="s">
         <v>78</v>
@@ -17034,16 +17220,16 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="13" t="s">
-        <v>772</v>
+        <v>784</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="C98" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="E98" s="15" t="s">
         <v>130</v>
@@ -17055,7 +17241,7 @@
         <v>120</v>
       </c>
       <c r="I98" s="16" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="K98" s="17" t="s">
         <v>78</v>
@@ -17085,7 +17271,7 @@
         <v>95</v>
       </c>
       <c r="T98" s="20" t="s">
-        <v>667</v>
+        <v>679</v>
       </c>
       <c r="U98" s="20" t="s">
         <v>166</v>
@@ -17103,13 +17289,13 @@
         <v>311</v>
       </c>
       <c r="AF98" s="24" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
       <c r="AG98" s="24" t="s">
         <v>8</v>
       </c>
       <c r="AH98" s="24" t="s">
-        <v>735</v>
+        <v>747</v>
       </c>
     </row>
     <row r="99" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17128,25 +17314,25 @@
       <c r="I99" s="41"/>
       <c r="J99" s="41"/>
       <c r="K99" s="42" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="L99" s="42" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="M99" s="42" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="N99" s="43"/>
       <c r="O99" s="43"/>
       <c r="P99" s="43"/>
       <c r="Q99" s="44" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="R99" s="44" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="S99" s="44" t="s">
-        <v>737</v>
+        <v>749</v>
       </c>
       <c r="T99" s="46"/>
       <c r="U99" s="46"/>
@@ -17166,34 +17352,34 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="13" t="s">
-        <v>773</v>
+        <v>785</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="D100" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E100" s="15" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="F100" s="15" t="s">
         <v>70</v>
       </c>
       <c r="G100" s="15" t="s">
-        <v>738</v>
+        <v>750</v>
       </c>
       <c r="H100" s="16" t="s">
-        <v>774</v>
+        <v>786</v>
       </c>
       <c r="I100" s="16" t="s">
         <v>6</v>
       </c>
       <c r="J100" s="16" t="s">
-        <v>774</v>
+        <v>786</v>
       </c>
       <c r="K100" s="66" t="s">
         <v>86</v>
@@ -17208,7 +17394,7 @@
         <v>16</v>
       </c>
       <c r="O100" s="60" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="P100" s="60" t="s">
         <v>16</v>
@@ -17217,7 +17403,7 @@
         <v>16</v>
       </c>
       <c r="R100" s="61" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="S100" s="61" t="s">
         <v>16</v>
@@ -17233,19 +17419,19 @@
         <v>542</v>
       </c>
       <c r="AC100" s="23" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="AD100" s="23" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="AE100" s="23" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="AF100" s="24" t="s">
         <v>18</v>
       </c>
       <c r="AG100" s="24" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="AH100" s="24" t="s">
         <v>18</v>
@@ -17254,7 +17440,7 @@
     <row r="101" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="38"/>
       <c r="B101" s="39" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
       <c r="C101" s="39"/>
       <c r="D101" s="39"/>
@@ -17280,10 +17466,10 @@
       <c r="R101" s="44"/>
       <c r="S101" s="44"/>
       <c r="T101" s="46" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="U101" s="46" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="V101" s="46"/>
       <c r="W101" s="47"/>
@@ -17301,13 +17487,13 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="s">
-        <v>776</v>
+        <v>788</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="D102" s="14" t="s">
         <v>10</v>
@@ -17316,19 +17502,19 @@
         <v>10</v>
       </c>
       <c r="F102" s="15" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="H102" s="16" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="I102" s="16" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="K102" s="17" t="s">
         <v>10</v>
       </c>
       <c r="L102" s="17" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="M102" s="17" t="s">
         <v>10</v>
@@ -17337,7 +17523,7 @@
         <v>10</v>
       </c>
       <c r="O102" s="18" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="P102" s="18" t="s">
         <v>10</v>
@@ -17346,7 +17532,7 @@
         <v>10</v>
       </c>
       <c r="R102" s="19" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="S102" s="19" t="s">
         <v>10</v>
@@ -17376,7 +17562,7 @@
         <v>10</v>
       </c>
       <c r="AG102" s="24" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="AH102" s="24" t="s">
         <v>10</v>
@@ -17385,14 +17571,14 @@
     <row r="103" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="38"/>
       <c r="B103" s="39" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="C103" s="39"/>
       <c r="D103" s="39" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="E103" s="40" t="s">
-        <v>695</v>
+        <v>707</v>
       </c>
       <c r="F103" s="40"/>
       <c r="G103" s="40"/>
@@ -17432,55 +17618,55 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="13" t="s">
-        <v>778</v>
+        <v>790</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="E104" s="15" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="F104" s="15" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="H104" s="16" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="I104" s="16" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="K104" s="17" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="L104" s="17" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="M104" s="17" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="N104" s="18" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="O104" s="18" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="P104" s="18" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="Q104" s="19" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="R104" s="19" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="S104" s="19" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="T104" s="20" t="s">
         <v>134</v>
@@ -17498,30 +17684,30 @@
         <v>306</v>
       </c>
       <c r="AD104" s="23" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="AE104" s="23" t="s">
         <v>306</v>
       </c>
       <c r="AF104" s="24" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="AG104" s="24" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="AH104" s="24" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
     </row>
     <row r="105" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="38"/>
       <c r="B105" s="39" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="C105" s="39"/>
       <c r="D105" s="39"/>
       <c r="E105" s="40" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="F105" s="40"/>
       <c r="G105" s="40"/>
@@ -17561,67 +17747,67 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="13" t="s">
-        <v>779</v>
+        <v>791</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="E106" s="15" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="F106" s="15" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="G106" s="15" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="H106" s="16" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="I106" s="16" t="s">
         <v>55</v>
       </c>
       <c r="K106" s="17" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="L106" s="17" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="M106" s="17" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="N106" s="18" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="O106" s="18" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="P106" s="18" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="Q106" s="19" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="R106" s="19" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="S106" s="19" t="s">
-        <v>748</v>
+        <v>760</v>
       </c>
       <c r="T106" s="20" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="U106" s="20" t="s">
-        <v>696</v>
+        <v>708</v>
       </c>
       <c r="V106" s="20" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="Z106" s="22" t="s">
         <v>527</v>
@@ -17639,18 +17825,18 @@
         <v>312</v>
       </c>
       <c r="AF106" s="24" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="AG106" s="24" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="AH106" s="24" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="14" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="Q107" s="19" t="s">
         <v>70</v>
@@ -17664,34 +17850,34 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="13" t="s">
-        <v>780</v>
+        <v>792</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="E108" s="15" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="F108" s="15" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="H108" s="16" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="I108" s="16" t="s">
-        <v>733</v>
+        <v>745</v>
       </c>
       <c r="AC108" s="23" t="s">
         <v>16</v>
       </c>
       <c r="AD108" s="23" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="AE108" s="23" t="s">
         <v>16</v>
@@ -17700,26 +17886,26 @@
     <row r="109" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="38"/>
       <c r="B109" s="39" t="s">
-        <v>781</v>
+        <v>793</v>
       </c>
       <c r="C109" s="39" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="D109" s="39" t="s">
-        <v>781</v>
+        <v>793</v>
       </c>
       <c r="E109" s="40" t="s">
-        <v>781</v>
+        <v>793</v>
       </c>
       <c r="F109" s="40" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="G109" s="40"/>
       <c r="H109" s="41" t="s">
-        <v>781</v>
+        <v>793</v>
       </c>
       <c r="I109" s="41" t="s">
-        <v>732</v>
+        <v>744</v>
       </c>
       <c r="J109" s="41"/>
       <c r="K109" s="42"/>
@@ -17750,103 +17936,103 @@
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="67"/>
       <c r="B110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="C110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="D110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="E110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="F110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="G110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="H110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="I110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="J110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="K110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="L110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="M110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="N110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="O110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="P110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="Q110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="R110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="S110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="T110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="U110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="V110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="W110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="X110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="Y110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="Z110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="AA110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="AB110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="AC110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="AD110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="AE110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="AF110" s="67" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="AG110" s="67" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="AH110" s="67" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17854,57 +18040,57 @@
       <c r="B111" s="67"/>
       <c r="C111" s="67"/>
       <c r="D111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="E111" s="67"/>
       <c r="F111" s="67"/>
       <c r="G111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="H111" s="67"/>
       <c r="I111" s="67"/>
       <c r="J111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="K111" s="67"/>
       <c r="L111" s="67"/>
       <c r="M111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="N111" s="67"/>
       <c r="O111" s="67"/>
       <c r="P111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="Q111" s="67"/>
       <c r="R111" s="67"/>
       <c r="S111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="T111" s="67"/>
       <c r="U111" s="67"/>
       <c r="V111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="W111" s="67"/>
       <c r="X111" s="67"/>
       <c r="Y111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="Z111" s="67"/>
       <c r="AA111" s="67"/>
       <c r="AB111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="AC111" s="67"/>
       <c r="AD111" s="67"/>
       <c r="AE111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="AF111" s="67"/>
       <c r="AG111" s="67"/>
       <c r="AH111" s="68" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17946,57 +18132,57 @@
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="67"/>
       <c r="B113" s="69" t="s">
-        <v>786</v>
+        <v>798</v>
       </c>
       <c r="C113" s="69"/>
       <c r="D113" s="69"/>
       <c r="E113" s="69" t="s">
-        <v>787</v>
+        <v>799</v>
       </c>
       <c r="F113" s="69"/>
       <c r="G113" s="69"/>
       <c r="H113" s="69" t="s">
-        <v>788</v>
+        <v>800</v>
       </c>
       <c r="I113" s="69"/>
       <c r="J113" s="69"/>
       <c r="K113" s="69" t="s">
-        <v>789</v>
+        <v>801</v>
       </c>
       <c r="L113" s="69"/>
       <c r="M113" s="69"/>
       <c r="N113" s="69" t="s">
-        <v>790</v>
+        <v>802</v>
       </c>
       <c r="O113" s="69"/>
       <c r="P113" s="69"/>
       <c r="Q113" s="69" t="s">
-        <v>791</v>
+        <v>803</v>
       </c>
       <c r="R113" s="69"/>
       <c r="S113" s="69"/>
       <c r="T113" s="69" t="s">
-        <v>792</v>
+        <v>804</v>
       </c>
       <c r="U113" s="69"/>
       <c r="V113" s="69"/>
       <c r="W113" s="69" t="s">
-        <v>793</v>
+        <v>805</v>
       </c>
       <c r="X113" s="69"/>
       <c r="Y113" s="69"/>
       <c r="Z113" s="69" t="s">
-        <v>794</v>
+        <v>806</v>
       </c>
       <c r="AA113" s="69"/>
       <c r="AB113" s="69"/>
       <c r="AC113" s="69" t="s">
-        <v>795</v>
+        <v>807</v>
       </c>
       <c r="AD113" s="69"/>
       <c r="AE113" s="69"/>
       <c r="AF113" s="69" t="s">
-        <v>796</v>
+        <v>808</v>
       </c>
       <c r="AG113" s="69"/>
       <c r="AH113" s="69"/>

</xml_diff>